<commit_message>
Frontend 23 and Updated Scrum Board
NA
</commit_message>
<xml_diff>
--- a/Scrum Board/Agile_Sprints.xlsx
+++ b/Scrum Board/Agile_Sprints.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NewGladiator\OnlineExam\Scrum Board\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160"/>
   </bookViews>
@@ -15,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -140,6 +135,60 @@
     </r>
   </si>
   <si>
+    <t>Project Name : Online Examination Portal</t>
+  </si>
+  <si>
+    <t>Team Lead</t>
+  </si>
+  <si>
+    <t>Saurav Tiwari</t>
+  </si>
+  <si>
+    <t>Team Members</t>
+  </si>
+  <si>
+    <t>Ajay Upadhyaya</t>
+  </si>
+  <si>
+    <t>Yogesh Narwal</t>
+  </si>
+  <si>
+    <t>Sonali Dudve</t>
+  </si>
+  <si>
+    <t>Task Completed(25/09)</t>
+  </si>
+  <si>
+    <t>1. Question Set Addition and Removal
+2. UI</t>
+  </si>
+  <si>
+    <t>1.  Admin Module
+2. Student Module</t>
+  </si>
+  <si>
+    <t>Task Completed(29/09)</t>
+  </si>
+  <si>
+    <t>Task Completed(27/09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verified</t>
+  </si>
+  <si>
+    <t>Verified</t>
+  </si>
+  <si>
+    <t>Task Completed (25/09)</t>
+  </si>
+  <si>
+    <t>Task Completed(01/10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Test Conduct
+2. </t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1. Add a constant theme for the web app with material design and constant headers and footers. </t>
     </r>
@@ -152,7 +201,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Sonali)</t>
+      <t>(Ajay &amp; Sonali)</t>
     </r>
     <r>
       <rPr>
@@ -207,7 +256,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-4. Searching and implementing best logic for "forgot password" option and captcha.</t>
+4. Searching and implementing best logic for "forgot password", "New User Registration" option and captcha.</t>
     </r>
     <r>
       <rPr>
@@ -222,36 +271,29 @@
     </r>
   </si>
   <si>
-    <t>Project Name : Online Examination Portal</t>
-  </si>
-  <si>
-    <t>Team Lead</t>
-  </si>
-  <si>
-    <t>Saurav Tiwari</t>
-  </si>
-  <si>
-    <t>Team Members</t>
-  </si>
-  <si>
-    <t>Ajay Upadhyaya</t>
-  </si>
-  <si>
-    <t>Yogesh Narwal</t>
-  </si>
-  <si>
-    <t>Sonali Dudve</t>
-  </si>
-  <si>
-    <t>Task Completed(25/09)</t>
-  </si>
-  <si>
-    <t>1. Question Set Addition and Removal
-2. UI</t>
-  </si>
-  <si>
-    <r>
-      <t>1. WebApi for Question Set addition and removal, their respective Sql table, components for admin model  (</t>
+    <r>
+      <t>1. WebApi for report and its filters,test and its filter (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yogesh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; </t>
     </r>
     <r>
       <rPr>
@@ -273,18 +315,18 @@
         <scheme val="minor"/>
       </rPr>
       <t>)
-2. UI (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ajay &amp; Sonali</t>
+2.Admin Dashboard, Report View, and graphical display of Score, Question Preparation, Save As PDF, Timer and Services (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Saurav,Ajay &amp; Sonali</t>
     </r>
     <r>
       <rPr>
@@ -306,6 +348,76 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Saurav &amp; Yogesh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Level 1,2 and 3 test FrontEnd (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ajay, Saurav and Sonali</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+2.Student Dashboard, Report View, and graphical display of Score, Take Exam (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Saurav &amp; Ajay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+3. Bug Fixing, Necessary Backend and Maintain Backup (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Yogesh</t>
     </r>
     <r>
@@ -320,33 +432,8 @@
     </r>
   </si>
   <si>
-    <t>1.  Admin Module
-2. Student Module</t>
-  </si>
-  <si>
-    <r>
-      <t>1. WebApi for report and its filters,test and its filter (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Yogesh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &amp; </t>
+    <r>
+      <t>1. WebApi for Question Set addition and removal, their respective Sql table, components for admin model  (</t>
     </r>
     <r>
       <rPr>
@@ -368,18 +455,18 @@
         <scheme val="minor"/>
       </rPr>
       <t>)
-2.Admin Dashboard, Report View, and graphical display of Score, Question Preparation, Save As PDF, and Timer (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Saurav,Ajay &amp; Sonali</t>
+2. User Interface Implementation in Angular for the Admin and Student Module. Also addition of corresponding Services for connecting with WebAPI and testing the wroking wrt to frontend. (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ajay &amp; Sonali</t>
     </r>
     <r>
       <rPr>
@@ -401,7 +488,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Saurav &amp; Yogesh</t>
+      <t>Yogesh</t>
     </r>
     <r>
       <rPr>
@@ -413,105 +500,13 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t>Task Completed(29/09)</t>
-  </si>
-  <si>
-    <t>Task Completed(27/09)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Verified</t>
-  </si>
-  <si>
-    <t>Verified</t>
-  </si>
-  <si>
-    <t>Task Completed (25/09)</t>
-  </si>
-  <si>
-    <r>
-      <t>1. Level 1,2 and 3 test FrontEnd (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ajay, Saurav and Sonali</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-2.Student Dashboard, Report View, and graphical display of Score, Take Exam (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Saurav,Ajay &amp; Sonali</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-3. Bug Fixing, Necessary Backend and Maintain Backup (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Yogesh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Task Completed(01/10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Test Conduct
-2. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -732,11 +727,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1046,39 +1041,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="78.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+    <row r="1" spans="1:6" ht="33" customHeight="1">
+      <c r="A1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="90" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1106,14 +1101,14 @@
         <v>6</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1123,103 +1118,103 @@
         <v>6</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="120">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90">
+      <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="74.45" customHeight="1">
       <c r="A7" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="74.45" customHeight="1">
       <c r="A8" s="14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>30</v>
       </c>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="C9" s="12"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="3"/>
       <c r="B11" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>